<commit_message>
little touches here and there
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\fc_hydro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DC13AA-E8E8-47CD-8AB8-049CDE331832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C81054B-DC3B-47D1-836F-A72721AE2AF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20070" yWindow="3060" windowWidth="15180" windowHeight="12870" xr2:uid="{7F61EDE7-CB94-45C5-83B8-2106FB1B135E}"/>
   </bookViews>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -476,7 +478,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
computation of the co2 emmisiions and subsidence in main.py according to Imam's formulas
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\blopti_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6E8504-56D3-4D57-9995-65DEF859783E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F2CEAD-3510-4DA5-8F45-8719E84FCC1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21765" yWindow="8145" windowWidth="7560" windowHeight="10050" xr2:uid="{7F61EDE7-CB94-45C5-83B8-2106FB1B135E}"/>
+    <workbookView xWindow="6405" yWindow="1095" windowWidth="17505" windowHeight="9330" xr2:uid="{7F61EDE7-CB94-45C5-83B8-2106FB1B135E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>WTD_input_and_output_folder</t>
   </si>
@@ -102,7 +104,34 @@
     <t>output/cwl_estimation</t>
   </si>
   <si>
-    <t>data/sum_canals_clip.tif</t>
+    <t>landcover</t>
+  </si>
+  <si>
+    <t>Needed for CO2 and subsidence rate calculation from WTD</t>
+  </si>
+  <si>
+    <t>canal_blocks_raster</t>
+  </si>
+  <si>
+    <t>data/blocks/canal_blocks.tif</t>
+  </si>
+  <si>
+    <t>Optional. Positions of canal blocks</t>
+  </si>
+  <si>
+    <t>sensor_locations</t>
+  </si>
+  <si>
+    <t>data/sensors/sensors.tif</t>
+  </si>
+  <si>
+    <t>Optional. Sensor locations</t>
+  </si>
+  <si>
+    <t>data/new_canal_raster/sum_canal_raster.tif</t>
+  </si>
+  <si>
+    <t>data/Landcover_2018/landcover.tif</t>
   </si>
 </sst>
 </file>
@@ -455,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F49BA472-FFBD-41DC-9472-8CD8ECD904A2}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +528,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -569,6 +598,39 @@
       </c>
       <c r="C11" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>